<commit_message>
x2 is the best
</commit_message>
<xml_diff>
--- a/4x4x4solver_v6/analytics.xlsx
+++ b/4x4x4solver_v6/analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\Solvour\4x4x4solver_v6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E32802-E231-4B54-8233-013F035824A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8F47DB-419E-4F86-A1CE-6949D5A593BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{946BFEEE-BBBF-4482-BF8B-5542A0A8C7AB}"/>
   </bookViews>
@@ -454,49 +454,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -5089,22 +5089,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -26736,10 +26736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C862F1A2-4B7F-4B62-84DD-D97E7C6441C1}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -26753,6 +26753,12 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>5.0672748089999997</v>
+      </c>
+      <c r="B2">
+        <v>58</v>
+      </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -26767,110 +26773,154 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>0.287303209</v>
+      </c>
+      <c r="B3">
+        <v>51</v>
+      </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="e">
+      <c r="E3">
         <f>AVERAGE(A:A)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" t="e">
+        <v>4.201494026139998</v>
+      </c>
+      <c r="F3">
         <f>AVERAGE(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>56.8</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="e">
+      <c r="I3">
         <f>COUNTIFS(A:A,"&lt;10")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>94</v>
       </c>
       <c r="J3">
         <f>COUNT(B:B)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>6.5067868229999997</v>
+      </c>
+      <c r="B4">
+        <v>61</v>
+      </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="e">
+      <c r="E4">
         <f>_xlfn.STDEV.S(A:A)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" t="e">
+        <v>3.1267812330311431</v>
+      </c>
+      <c r="F4">
         <f>_xlfn.STDEV.S(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>2.5346089292516951</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="e">
+      <c r="I4">
         <f>COUNTIFS(A:A,"&lt;5")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>1.440039635</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5">
         <f>MAX(A:A)</f>
-        <v>0</v>
+        <v>14.11067486</v>
       </c>
       <c r="F5">
         <f>MAX(B:B)</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="e">
+      <c r="I5">
         <f>COUNTIFS(A:A,"&lt;3")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>0.66227531399999995</v>
+      </c>
+      <c r="B6">
+        <v>53</v>
+      </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="e">
+      <c r="E6">
         <f>MEDIAN(A:A)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F6" t="e">
+        <v>3.7392941715000001</v>
+      </c>
+      <c r="F6">
         <f>MEDIAN(B:B)</f>
-        <v>#NUM!</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="e">
+      <c r="I6">
         <f>COUNTIFS(A:A,"&lt;2")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>0.92621779400000004</v>
+      </c>
+      <c r="B7">
+        <v>53</v>
+      </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7">
         <f>MIN(A:A)</f>
-        <v>0</v>
+        <v>0.23536992100000001</v>
       </c>
       <c r="F7">
         <f>MIN(B:B)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="e">
+      <c r="I7">
         <f>COUNTIFS(A:A,"&lt;1")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>2.8318591120000001</v>
+      </c>
+      <c r="B8">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>1.5928866859999999</v>
+      </c>
+      <c r="B9">
+        <v>56</v>
+      </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -26879,6 +26929,12 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>5.0022780899999999</v>
+      </c>
+      <c r="B10">
+        <v>58</v>
+      </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
@@ -26899,6 +26955,12 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>5.3004183769999997</v>
+      </c>
+      <c r="B11">
+        <v>55</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
@@ -26907,7 +26969,7 @@
       </c>
       <c r="F11">
         <f>COUNTIFS(A:A,"&lt;"&amp;E11,A:A,"&gt;="&amp;D11)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>48</v>
@@ -26921,6 +26983,12 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>6.6854703430000004</v>
+      </c>
+      <c r="B12">
+        <v>57</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -26929,7 +26997,7 @@
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F41" si="1">COUNTIFS(A:A,"&lt;"&amp;E12,A:A,"&gt;="&amp;D12)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H12">
         <v>50</v>
@@ -26939,10 +27007,16 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2.9165472979999998</v>
+      </c>
+      <c r="B13">
+        <v>56</v>
+      </c>
       <c r="D13">
         <v>2</v>
       </c>
@@ -26951,7 +27025,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>52</v>
@@ -26961,10 +27035,16 @@
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>1.670004606</v>
+      </c>
+      <c r="B14">
+        <v>55</v>
+      </c>
       <c r="D14">
         <v>3</v>
       </c>
@@ -26973,7 +27053,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H14">
         <v>54</v>
@@ -26983,10 +27063,16 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>8.2502539160000001</v>
+      </c>
+      <c r="B15">
+        <v>58</v>
+      </c>
       <c r="D15">
         <v>4</v>
       </c>
@@ -26995,7 +27081,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H15">
         <v>56</v>
@@ -27005,10 +27091,16 @@
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>11.188903809999999</v>
+      </c>
+      <c r="B16">
+        <v>61</v>
+      </c>
       <c r="D16">
         <v>5</v>
       </c>
@@ -27017,7 +27109,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H16">
         <v>58</v>
@@ -27027,10 +27119,16 @@
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>0.74304985999999995</v>
+      </c>
+      <c r="B17">
+        <v>53</v>
+      </c>
       <c r="D17">
         <v>6</v>
       </c>
@@ -27039,7 +27137,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H17">
         <v>60</v>
@@ -27049,10 +27147,16 @@
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>0.71809864000000001</v>
+      </c>
+      <c r="B18">
+        <v>54</v>
+      </c>
       <c r="D18">
         <v>7</v>
       </c>
@@ -27061,7 +27165,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <v>62</v>
@@ -27074,7 +27178,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>8.778671503</v>
+      </c>
+      <c r="B19">
+        <v>61</v>
+      </c>
       <c r="D19">
         <v>8</v>
       </c>
@@ -27083,10 +27193,16 @@
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>4.8911504749999999</v>
+      </c>
+      <c r="B20">
+        <v>58</v>
+      </c>
       <c r="D20">
         <v>9</v>
       </c>
@@ -27095,10 +27211,16 @@
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>2.9650721550000001</v>
+      </c>
+      <c r="B21">
+        <v>58</v>
+      </c>
       <c r="D21">
         <v>10</v>
       </c>
@@ -27110,7 +27232,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>1.9836964610000001</v>
+      </c>
+      <c r="B22">
+        <v>53</v>
+      </c>
       <c r="D22">
         <v>11</v>
       </c>
@@ -27119,10 +27247,16 @@
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>3.5445199010000001</v>
+      </c>
+      <c r="B23">
+        <v>54</v>
+      </c>
       <c r="D23">
         <v>12</v>
       </c>
@@ -27134,7 +27268,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>2.8025181290000001</v>
+      </c>
+      <c r="B24">
+        <v>57</v>
+      </c>
       <c r="D24">
         <v>13</v>
       </c>
@@ -27143,10 +27283,16 @@
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>4.4311487669999998</v>
+      </c>
+      <c r="B25">
+        <v>58</v>
+      </c>
       <c r="D25">
         <v>14</v>
       </c>
@@ -27155,10 +27301,16 @@
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>4.1358075139999997</v>
+      </c>
+      <c r="B26">
+        <v>55</v>
+      </c>
       <c r="D26">
         <v>15</v>
       </c>
@@ -27170,7 +27322,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>7.7010188099999999</v>
+      </c>
+      <c r="B27">
+        <v>58</v>
+      </c>
       <c r="D27">
         <v>16</v>
       </c>
@@ -27182,7 +27340,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>3.8961384300000002</v>
+      </c>
+      <c r="B28">
+        <v>61</v>
+      </c>
       <c r="D28">
         <v>17</v>
       </c>
@@ -27194,7 +27358,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>4.2017691140000002</v>
+      </c>
+      <c r="B29">
+        <v>58</v>
+      </c>
       <c r="D29">
         <v>18</v>
       </c>
@@ -27206,7 +27376,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>1.5299046039999999</v>
+      </c>
+      <c r="B30">
+        <v>55</v>
+      </c>
       <c r="D30">
         <v>19</v>
       </c>
@@ -27218,7 +27394,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>11.08447003</v>
+      </c>
+      <c r="B31">
+        <v>60</v>
+      </c>
       <c r="D31">
         <v>20</v>
       </c>
@@ -27230,7 +27412,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>1.7592420580000001</v>
+      </c>
+      <c r="B32">
+        <v>54</v>
+      </c>
       <c r="D32">
         <v>21</v>
       </c>
@@ -27242,7 +27430,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>3.7530398370000002</v>
+      </c>
+      <c r="B33">
+        <v>58</v>
+      </c>
       <c r="D33">
         <v>22</v>
       </c>
@@ -27254,7 +27448,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>3.5784304140000001</v>
+      </c>
+      <c r="B34">
+        <v>56</v>
+      </c>
       <c r="D34">
         <v>23</v>
       </c>
@@ -27266,7 +27466,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>5.8275206089999996</v>
+      </c>
+      <c r="B35">
+        <v>56</v>
+      </c>
       <c r="D35">
         <v>24</v>
       </c>
@@ -27278,7 +27484,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>0.94942855800000003</v>
+      </c>
+      <c r="B36">
+        <v>52</v>
+      </c>
       <c r="D36">
         <v>25</v>
       </c>
@@ -27290,7 +27502,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>2.0784864430000001</v>
+      </c>
+      <c r="B37">
+        <v>56</v>
+      </c>
       <c r="D37">
         <v>26</v>
       </c>
@@ -27302,7 +27520,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>2.5875957010000001</v>
+      </c>
+      <c r="B38">
+        <v>59</v>
+      </c>
       <c r="D38">
         <v>27</v>
       </c>
@@ -27314,7 +27538,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>1.6236579419999999</v>
+      </c>
+      <c r="B39">
+        <v>58</v>
+      </c>
       <c r="D39">
         <v>28</v>
       </c>
@@ -27326,7 +27556,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>1.0193178650000001</v>
+      </c>
+      <c r="B40">
+        <v>52</v>
+      </c>
       <c r="D40">
         <v>29</v>
       </c>
@@ -27338,7 +27574,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>1.732247353</v>
+      </c>
+      <c r="B41">
+        <v>54</v>
+      </c>
       <c r="D41">
         <v>30</v>
       </c>
@@ -27348,6 +27590,486 @@
       <c r="F41">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>3.834183216</v>
+      </c>
+      <c r="B42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>2.8641924859999999</v>
+      </c>
+      <c r="B43">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>13.00402379</v>
+      </c>
+      <c r="B44">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>3.7727608680000002</v>
+      </c>
+      <c r="B45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>8.5419690609999996</v>
+      </c>
+      <c r="B46">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>0.66023397399999995</v>
+      </c>
+      <c r="B47">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>4.0819411280000004</v>
+      </c>
+      <c r="B48">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>9.46049118</v>
+      </c>
+      <c r="B49">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>7.0185046199999999</v>
+      </c>
+      <c r="B50">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>1.6422502990000001</v>
+      </c>
+      <c r="B51">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>3.1352026460000002</v>
+      </c>
+      <c r="B52">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>1.2506206040000001</v>
+      </c>
+      <c r="B53">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>3.9224591260000001</v>
+      </c>
+      <c r="B54">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>7.8286769390000002</v>
+      </c>
+      <c r="B55">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>4.3092212679999999</v>
+      </c>
+      <c r="B56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>7.0957560539999998</v>
+      </c>
+      <c r="B57">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>0.31914639500000003</v>
+      </c>
+      <c r="B58">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>3.4268589020000002</v>
+      </c>
+      <c r="B59">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>3.2952854629999999</v>
+      </c>
+      <c r="B60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>2.42135334</v>
+      </c>
+      <c r="B61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>1.662703037</v>
+      </c>
+      <c r="B62">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>3.982432604</v>
+      </c>
+      <c r="B63">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>4.0896730420000003</v>
+      </c>
+      <c r="B64">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>0.23536992100000001</v>
+      </c>
+      <c r="B65">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>5.5029833320000003</v>
+      </c>
+      <c r="B66">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>5.9727659229999999</v>
+      </c>
+      <c r="B67">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>4.0769577029999997</v>
+      </c>
+      <c r="B68">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>2.5970783229999999</v>
+      </c>
+      <c r="B69">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>8.9266226290000006</v>
+      </c>
+      <c r="B70">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>11.640734670000001</v>
+      </c>
+      <c r="B71">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>1.3334331509999999</v>
+      </c>
+      <c r="B72">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>3.6005725860000002</v>
+      </c>
+      <c r="B73">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>4.4960887429999996</v>
+      </c>
+      <c r="B74">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>0.41588640199999999</v>
+      </c>
+      <c r="B75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>1.0907924179999999</v>
+      </c>
+      <c r="B76">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>13.147104499999999</v>
+      </c>
+      <c r="B77">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>4.2637541289999996</v>
+      </c>
+      <c r="B78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>5.8724448679999997</v>
+      </c>
+      <c r="B79">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>4.4637324810000001</v>
+      </c>
+      <c r="B80">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>1.2601177690000001</v>
+      </c>
+      <c r="B81">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>6.7468934059999999</v>
+      </c>
+      <c r="B82">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>4.8749299050000001</v>
+      </c>
+      <c r="B83">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>1.568384886</v>
+      </c>
+      <c r="B84">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>1.463377476</v>
+      </c>
+      <c r="B85">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>14.11067486</v>
+      </c>
+      <c r="B86">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>1.2223513130000001</v>
+      </c>
+      <c r="B87">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>2.9281678200000001</v>
+      </c>
+      <c r="B88">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>1.8511536120000001</v>
+      </c>
+      <c r="B89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>3.5030717849999999</v>
+      </c>
+      <c r="B90">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A91">
+        <v>1.0013461109999999</v>
+      </c>
+      <c r="B91">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>5.432256937</v>
+      </c>
+      <c r="B92">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A93">
+        <v>1.702488899</v>
+      </c>
+      <c r="B93">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A94">
+        <v>6.574088573</v>
+      </c>
+      <c r="B94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A95">
+        <v>1.4726161959999999</v>
+      </c>
+      <c r="B95">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A96">
+        <v>8.6567151550000005</v>
+      </c>
+      <c r="B96">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A97">
+        <v>9.2558860779999996</v>
+      </c>
+      <c r="B97">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A98">
+        <v>6.6203200820000001</v>
+      </c>
+      <c r="B98">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A99">
+        <v>3.8141021730000002</v>
+      </c>
+      <c r="B99">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A100">
+        <v>4.4641282560000004</v>
+      </c>
+      <c r="B100">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A101">
+        <v>3.725548506</v>
+      </c>
+      <c r="B101">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -32062,7 +32784,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="D30" sqref="D30:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
1.6-1.9 is the best
</commit_message>
<xml_diff>
--- a/4x4x4solver_v6/analytics.xlsx
+++ b/4x4x4solver_v6/analytics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\Solvour\4x4x4solver_v6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CA49F4-40D2-4510-BB36-8F4E97E65348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF5181D-10BD-4C76-B205-BF896BE667CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{946BFEEE-BBBF-4482-BF8B-5542A0A8C7AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{946BFEEE-BBBF-4482-BF8B-5542A0A8C7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="NyanyanFunc_-1.4-1.7事前計算_2" sheetId="22" r:id="rId1"/>
@@ -424,43 +424,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -4927,22 +4927,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -44412,10 +44412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FA8839-989C-4FA1-9500-8CF631A1A399}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -44429,6 +44429,12 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2.4515888690000001</v>
+      </c>
+      <c r="B2">
+        <v>58</v>
+      </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -44443,110 +44449,154 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2.1546518799999999</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="e">
+      <c r="E3">
         <f>AVERAGE(A:A)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" t="e">
+        <v>3.6783045721300001</v>
+      </c>
+      <c r="F3">
         <f>AVERAGE(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>57.03</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="e">
+      <c r="I3">
         <f>COUNTIFS(A:A,"&lt;10")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>97</v>
       </c>
       <c r="J3">
         <f>COUNT(B:B)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3.260409594</v>
+      </c>
+      <c r="B4">
+        <v>57</v>
+      </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="e">
+      <c r="E4">
         <f>_xlfn.STDEV.S(A:A)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" t="e">
+        <v>2.3726720710986329</v>
+      </c>
+      <c r="F4">
         <f>_xlfn.STDEV.S(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>1.9040361171347397</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="e">
+      <c r="I4">
         <f>COUNTIFS(A:A,"&lt;5")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>2.731681585</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5">
         <f>MAX(A:A)</f>
-        <v>0</v>
+        <v>12.24881053</v>
       </c>
       <c r="F5">
         <f>MAX(B:B)</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="e">
+      <c r="I5">
         <f>COUNTIFS(A:A,"&lt;3")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>2.1213302610000002</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="e">
+      <c r="E6">
         <f>MEDIAN(A:A)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F6" t="e">
+        <v>3.0517278909999996</v>
+      </c>
+      <c r="F6">
         <f>MEDIAN(B:B)</f>
-        <v>#NUM!</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="e">
+      <c r="I6">
         <f>COUNTIFS(A:A,"&lt;2")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>2.5203077789999999</v>
+      </c>
+      <c r="B7">
+        <v>59</v>
+      </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7">
         <f>MIN(A:A)</f>
-        <v>0</v>
+        <v>0.57909440999999995</v>
       </c>
       <c r="F7">
         <f>MIN(B:B)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="e">
+      <c r="I7">
         <f>COUNTIFS(A:A,"&lt;1")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>7.0000000000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>3.562074661</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>1.1778507229999999</v>
+      </c>
+      <c r="B9">
+        <v>54</v>
+      </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -44555,6 +44605,12 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>3.725240946</v>
+      </c>
+      <c r="B10">
+        <v>57</v>
+      </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
@@ -44575,6 +44631,12 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2.7826612000000002</v>
+      </c>
+      <c r="B11">
+        <v>56</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
@@ -44583,7 +44645,7 @@
       </c>
       <c r="F11">
         <f>COUNTIFS(A:A,"&lt;"&amp;E11,A:A,"&gt;="&amp;D11)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <v>48</v>
@@ -44597,6 +44659,12 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2.1442692280000002</v>
+      </c>
+      <c r="B12">
+        <v>61</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -44605,7 +44673,7 @@
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F28" si="1">COUNTIFS(A:A,"&lt;"&amp;E12,A:A,"&gt;="&amp;D12)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H12">
         <v>50</v>
@@ -44619,6 +44687,12 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>7.6136541370000002</v>
+      </c>
+      <c r="B13">
+        <v>55</v>
+      </c>
       <c r="D13">
         <v>2</v>
       </c>
@@ -44627,7 +44701,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H13">
         <v>52</v>
@@ -44637,10 +44711,16 @@
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>3.0261642929999999</v>
+      </c>
+      <c r="B14">
+        <v>58</v>
+      </c>
       <c r="D14">
         <v>3</v>
       </c>
@@ -44649,7 +44729,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H14">
         <v>54</v>
@@ -44659,10 +44739,16 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>0.96350955999999999</v>
+      </c>
+      <c r="B15">
+        <v>56</v>
+      </c>
       <c r="D15">
         <v>4</v>
       </c>
@@ -44671,7 +44757,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H15">
         <v>56</v>
@@ -44681,10 +44767,16 @@
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2.471803188</v>
+      </c>
+      <c r="B16">
+        <v>57</v>
+      </c>
       <c r="D16">
         <v>5</v>
       </c>
@@ -44693,7 +44785,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16">
         <v>58</v>
@@ -44703,10 +44795,16 @@
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>10.840979340000001</v>
+      </c>
+      <c r="B17">
+        <v>57</v>
+      </c>
       <c r="D17">
         <v>6</v>
       </c>
@@ -44715,7 +44813,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <v>60</v>
@@ -44725,10 +44823,16 @@
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>3.0772914889999998</v>
+      </c>
+      <c r="B18">
+        <v>57</v>
+      </c>
       <c r="D18">
         <v>7</v>
       </c>
@@ -44737,7 +44841,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <v>62</v>
@@ -44747,10 +44851,16 @@
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>0.65652632700000002</v>
+      </c>
+      <c r="B19">
+        <v>55</v>
+      </c>
       <c r="D19">
         <v>8</v>
       </c>
@@ -44759,10 +44869,16 @@
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>5.275809765</v>
+      </c>
+      <c r="B20">
+        <v>57</v>
+      </c>
       <c r="D20">
         <v>9</v>
       </c>
@@ -44771,10 +44887,16 @@
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>2.960633278</v>
+      </c>
+      <c r="B21">
+        <v>58</v>
+      </c>
       <c r="D21">
         <v>10</v>
       </c>
@@ -44783,10 +44905,16 @@
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>0.79542064700000004</v>
+      </c>
+      <c r="B22">
+        <v>57</v>
+      </c>
       <c r="D22">
         <v>11</v>
       </c>
@@ -44798,7 +44926,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>2.6291480059999999</v>
+      </c>
+      <c r="B23">
+        <v>59</v>
+      </c>
       <c r="D23">
         <v>12</v>
       </c>
@@ -44807,10 +44941,16 @@
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>3.1703531740000002</v>
+      </c>
+      <c r="B24">
+        <v>55</v>
+      </c>
       <c r="D24">
         <v>13</v>
       </c>
@@ -44822,7 +44962,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>1.774428844</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
       <c r="D25">
         <v>14</v>
       </c>
@@ -44834,7 +44980,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>9.1141209599999993</v>
+      </c>
+      <c r="B26">
+        <v>57</v>
+      </c>
       <c r="D26">
         <v>15</v>
       </c>
@@ -44846,7 +44998,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>4.6597785949999997</v>
+      </c>
+      <c r="B27">
+        <v>58</v>
+      </c>
       <c r="D27">
         <v>16</v>
       </c>
@@ -44858,7 +45016,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>4.5995910169999998</v>
+      </c>
+      <c r="B28">
+        <v>56</v>
+      </c>
       <c r="D28">
         <v>17</v>
       </c>
@@ -44868,6 +45032,590 @@
       <c r="F28">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>4.5271880629999997</v>
+      </c>
+      <c r="B29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>2.5269479750000001</v>
+      </c>
+      <c r="B30">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>3.8092346190000002</v>
+      </c>
+      <c r="B31">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>7.77259016</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>3.7475244999999999</v>
+      </c>
+      <c r="B33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>1.72602129</v>
+      </c>
+      <c r="B34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>2.9609940049999999</v>
+      </c>
+      <c r="B35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>0.57909440999999995</v>
+      </c>
+      <c r="B36">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>2.6281774040000001</v>
+      </c>
+      <c r="B37">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>1.8581352229999999</v>
+      </c>
+      <c r="B38">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>10.24316597</v>
+      </c>
+      <c r="B39">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>7.0404469970000001</v>
+      </c>
+      <c r="B40">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>2.4019846920000001</v>
+      </c>
+      <c r="B41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>3.709634066</v>
+      </c>
+      <c r="B42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>3.5950248239999998</v>
+      </c>
+      <c r="B43">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>2.556922674</v>
+      </c>
+      <c r="B44">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>4.4183168410000002</v>
+      </c>
+      <c r="B45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>7.7683117389999996</v>
+      </c>
+      <c r="B46">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>4.3691461089999999</v>
+      </c>
+      <c r="B47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>4.2165665629999998</v>
+      </c>
+      <c r="B48">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>2.5098643300000001</v>
+      </c>
+      <c r="B49">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>2.7896647450000001</v>
+      </c>
+      <c r="B50">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>9.4240822790000003</v>
+      </c>
+      <c r="B51">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>4.3117578029999999</v>
+      </c>
+      <c r="B52">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>0.89023566200000004</v>
+      </c>
+      <c r="B53">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>4.7102961539999999</v>
+      </c>
+      <c r="B54">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>3.4129886630000001</v>
+      </c>
+      <c r="B55">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>3.766940355</v>
+      </c>
+      <c r="B56">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>1.4267148970000001</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>3.0175063610000001</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>3.9525747299999998</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>1.4027543069999999</v>
+      </c>
+      <c r="B60">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>4.7620477680000004</v>
+      </c>
+      <c r="B61">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>1.0964453220000001</v>
+      </c>
+      <c r="B62">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>3.0116739269999999</v>
+      </c>
+      <c r="B63">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>5.7808461189999996</v>
+      </c>
+      <c r="B64">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>6.7294251919999999</v>
+      </c>
+      <c r="B65">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>2.9786746499999999</v>
+      </c>
+      <c r="B66">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>4.4211430549999999</v>
+      </c>
+      <c r="B67">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>2.099215746</v>
+      </c>
+      <c r="B68">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>6.5132040980000001</v>
+      </c>
+      <c r="B69">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>1.5933530330000001</v>
+      </c>
+      <c r="B70">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>3.4521808620000001</v>
+      </c>
+      <c r="B71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>0.82740712199999999</v>
+      </c>
+      <c r="B72">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>1.529761076</v>
+      </c>
+      <c r="B73">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>6.2995972629999999</v>
+      </c>
+      <c r="B74">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>3.7860686779999999</v>
+      </c>
+      <c r="B75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>5.879130602</v>
+      </c>
+      <c r="B76">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>1.8154218200000001</v>
+      </c>
+      <c r="B77">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>4.5536518099999999</v>
+      </c>
+      <c r="B78">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>4.7544922830000003</v>
+      </c>
+      <c r="B79">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>3.86191678</v>
+      </c>
+      <c r="B80">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>2.015751839</v>
+      </c>
+      <c r="B81">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>2.1316390040000002</v>
+      </c>
+      <c r="B82">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>3.2462432379999999</v>
+      </c>
+      <c r="B83">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>2.763128042</v>
+      </c>
+      <c r="B84">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>1.1760563850000001</v>
+      </c>
+      <c r="B85">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>8.2255825999999992</v>
+      </c>
+      <c r="B86">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>2.2663700580000001</v>
+      </c>
+      <c r="B87">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>0.86867713899999999</v>
+      </c>
+      <c r="B88">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>12.24881053</v>
+      </c>
+      <c r="B89">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>2.7447051999999998</v>
+      </c>
+      <c r="B90">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A91">
+        <v>2.4633190630000001</v>
+      </c>
+      <c r="B91">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>4.1672286989999998</v>
+      </c>
+      <c r="B92">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A93">
+        <v>1.7526273729999999</v>
+      </c>
+      <c r="B93">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A94">
+        <v>2.1542541979999998</v>
+      </c>
+      <c r="B94">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A95">
+        <v>4.2349104879999997</v>
+      </c>
+      <c r="B95">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A96">
+        <v>3.1156010630000002</v>
+      </c>
+      <c r="B96">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A97">
+        <v>1.6279907229999999</v>
+      </c>
+      <c r="B97">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A98">
+        <v>3.1475281719999999</v>
+      </c>
+      <c r="B98">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A99">
+        <v>1.547876596</v>
+      </c>
+      <c r="B99">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A100">
+        <v>9.6197710040000004</v>
+      </c>
+      <c r="B100">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A101">
+        <v>4.2346408369999997</v>
+      </c>
+      <c r="B101">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -62394,8 +63142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BA33B1-CE5D-476B-8572-F81954994F4A}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -62652,7 +63400,7 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F28" si="1">COUNTIFS(A:A,"&lt;"&amp;E12,A:A,"&gt;="&amp;D12)</f>
+        <f t="shared" ref="F12:F27" si="1">COUNTIFS(A:A,"&lt;"&amp;E12,A:A,"&gt;="&amp;D12)</f>
         <v>29</v>
       </c>
       <c r="H12">

</xml_diff>